<commit_message>
latest health excel file
</commit_message>
<xml_diff>
--- a/resources/quality_of_life/diabetes_self_report/diabetes_self_report_processed_2023.xlsx
+++ b/resources/quality_of_life/diabetes_self_report/diabetes_self_report_processed_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damonmccullough/github/db-equitable-development-tool/resources/quality_of_life/diabetes_self_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3B90C7-D265-0443-8968-10766D1B1DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A44FAC-5B22-6040-BD49-2BC7F0312B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32120" yWindow="-3100" windowWidth="29040" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31900" yWindow="-3100" windowWidth="29040" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCHP_Diabetes_SelfRepHealth" sheetId="6" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -670,7 +670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -719,12 +719,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -739,21 +733,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -811,6 +790,30 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12"/>
@@ -4230,28 +4233,23 @@
       <c r="A67" s="1"/>
     </row>
     <row r="69" spans="1:15" ht="25.5" customHeight="1">
-      <c r="A69" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-      <c r="L69" s="18"/>
-      <c r="M69" s="18"/>
-      <c r="N69" s="18"/>
-      <c r="O69" s="18"/>
+      <c r="A69" s="68"/>
+      <c r="B69" s="68"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="68"/>
+      <c r="H69" s="68"/>
+      <c r="I69" s="68"/>
+      <c r="J69" s="68"/>
+      <c r="K69" s="68"/>
+      <c r="L69" s="68"/>
+      <c r="M69" s="68"/>
+      <c r="N69" s="68"/>
+      <c r="O69" s="68"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A69:O69"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4286,26 +4284,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="35.25" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7430,23 +7428,23 @@
       <c r="A73" s="1"/>
     </row>
     <row r="75" spans="1:15" ht="25.5" customHeight="1">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="18"/>
-      <c r="L75" s="18"/>
-      <c r="M75" s="18"/>
-      <c r="N75" s="18"/>
-      <c r="O75" s="18"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="61"/>
+      <c r="G75" s="61"/>
+      <c r="H75" s="61"/>
+      <c r="I75" s="61"/>
+      <c r="J75" s="61"/>
+      <c r="K75" s="61"/>
+      <c r="L75" s="61"/>
+      <c r="M75" s="61"/>
+      <c r="N75" s="61"/>
+      <c r="O75" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7461,7 +7459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06904A75-F3E9-5846-B1B7-7F6541B0232E}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -7469,1541 +7467,1541 @@
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="27" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="25" customWidth="1"/>
     <col min="4" max="4" width="3.33203125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="7" width="13.5" style="27" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="25" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="24" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="30.75" customHeight="1">
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="27" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="33" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="41">
+      <c r="A10" s="34">
         <v>101</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="36">
         <v>3.4</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="25">
         <v>1.9</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="25">
         <v>6</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="37">
         <f>ROUND(C10,0)</f>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="41">
+      <c r="A11" s="34">
         <v>102</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="36">
         <v>3.4</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="25">
         <v>1.9</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="25">
         <v>6</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="37">
         <f t="shared" ref="H11:H74" si="0">ROUND(C11,0)</f>
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="41">
+      <c r="A12" s="34">
         <v>103</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="36">
         <v>10.7</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="25">
         <v>7.7</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="25">
         <v>14.8</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="41">
+      <c r="A13" s="34">
         <v>104</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="36">
         <v>5</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="25">
         <v>3.2</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="25">
         <v>7.8</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="37">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="41">
+      <c r="A14" s="34">
         <v>105</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="36">
         <v>5</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="25">
         <v>3.2</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="25">
         <v>7.8</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="37">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="41">
+      <c r="A15" s="34">
         <v>106</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="36">
         <v>4</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="25">
         <v>2.4</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="25">
         <v>6.3</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="37">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="41">
+      <c r="A16" s="34">
         <v>107</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="36">
         <v>5.3</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="25">
         <v>3.1</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="25">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="37">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="41">
+      <c r="A17" s="34">
         <v>108</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="36">
         <v>3.6</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="25">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="25">
         <v>5.9</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="37">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="41">
+      <c r="A18" s="34">
         <v>109</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="36">
         <v>9.6</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="25">
         <v>6.7</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="25">
         <v>13.5</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="37">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="41">
+      <c r="A19" s="34">
         <v>110</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="36">
         <v>12.2</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="25">
         <v>9</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="25">
         <v>16.2</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="41">
+      <c r="A20" s="34">
         <v>111</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="36">
         <v>16.5</v>
       </c>
       <c r="D20" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="25">
         <v>12.5</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="25">
         <v>21.6</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="37">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="41">
+      <c r="A21" s="34">
         <v>112</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="36">
         <v>12.9</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="25">
         <v>9.6</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="25">
         <v>17.100000000000001</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="41">
+      <c r="A22" s="34">
         <v>201</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="36">
         <v>20.399999999999999</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="25">
         <v>15.4</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="25">
         <v>26.6</v>
       </c>
-      <c r="H22" s="44">
+      <c r="H22" s="37">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="41">
+      <c r="A23" s="34">
         <v>202</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="36">
         <v>20.399999999999999</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="25">
         <v>15.4</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="25">
         <v>26.6</v>
       </c>
-      <c r="H23" s="44">
+      <c r="H23" s="37">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="41">
+      <c r="A24" s="34">
         <v>203</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="36">
         <v>22</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="25">
         <v>17.8</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="25">
         <v>26.9</v>
       </c>
-      <c r="H24" s="44">
+      <c r="H24" s="37">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="41">
+      <c r="A25" s="34">
         <v>204</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="36">
         <v>16.899999999999999</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="25">
         <v>12.6</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="25">
         <v>22.4</v>
       </c>
-      <c r="H25" s="44">
+      <c r="H25" s="37">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="41">
+      <c r="A26" s="34">
         <v>205</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="36">
         <v>15.8</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="25">
         <v>11.7</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="25">
         <v>21.1</v>
       </c>
-      <c r="H26" s="44">
+      <c r="H26" s="37">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="41">
+      <c r="A27" s="34">
         <v>206</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="36">
         <v>22</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="25">
         <v>17.8</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="25">
         <v>26.9</v>
       </c>
-      <c r="H27" s="44">
+      <c r="H27" s="37">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="41">
+      <c r="A28" s="34">
         <v>207</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="36">
         <v>18.5</v>
       </c>
       <c r="D28" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="25">
         <v>14.3</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="25">
         <v>23.7</v>
       </c>
-      <c r="H28" s="44">
+      <c r="H28" s="37">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="41">
+      <c r="A29" s="34">
         <v>208</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="36">
         <v>12.3</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="25">
         <v>7.3</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="25">
         <v>19.899999999999999</v>
       </c>
-      <c r="H29" s="44">
+      <c r="H29" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="41">
+      <c r="A30" s="34">
         <v>209</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="36">
         <v>15.6</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="25">
         <v>11.8</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="25">
         <v>20.5</v>
       </c>
-      <c r="H30" s="44">
+      <c r="H30" s="37">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="41">
+      <c r="A31" s="34">
         <v>210</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="36">
         <v>13.4</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="25">
         <v>10</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="25">
         <v>17.899999999999999</v>
       </c>
-      <c r="H31" s="44">
+      <c r="H31" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="41">
+      <c r="A32" s="34">
         <v>211</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="36">
         <v>13.5</v>
       </c>
       <c r="D32" t="s">
         <v>107</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="25">
         <v>9.9</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="25">
         <v>18.2</v>
       </c>
-      <c r="H32" s="44">
+      <c r="H32" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="41">
+      <c r="A33" s="34">
         <v>212</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="36">
         <v>14.1</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="25">
         <v>10.7</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="25">
         <v>18.3</v>
       </c>
-      <c r="H33" s="44">
+      <c r="H33" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="41">
+      <c r="A34" s="34">
         <v>301</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="36">
         <v>11.1</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="25">
         <v>7.8</v>
       </c>
-      <c r="G34" s="27">
+      <c r="G34" s="25">
         <v>15.7</v>
       </c>
-      <c r="H34" s="44">
+      <c r="H34" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="41">
+      <c r="A35" s="34">
         <v>302</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="36">
         <v>6</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="25">
         <v>3.6</v>
       </c>
-      <c r="G35" s="27">
+      <c r="G35" s="25">
         <v>9.9</v>
       </c>
-      <c r="H35" s="44">
+      <c r="H35" s="37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="41">
+      <c r="A36" s="34">
         <v>303</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="36">
         <v>13.2</v>
       </c>
-      <c r="F36" s="27">
+      <c r="F36" s="25">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G36" s="27">
+      <c r="G36" s="25">
         <v>17.8</v>
       </c>
-      <c r="H36" s="44">
+      <c r="H36" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="41">
+      <c r="A37" s="34">
         <v>304</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="36">
         <v>13.1</v>
       </c>
-      <c r="F37" s="27">
+      <c r="F37" s="25">
         <v>9.5</v>
       </c>
-      <c r="G37" s="27">
+      <c r="G37" s="25">
         <v>17.8</v>
       </c>
-      <c r="H37" s="44">
+      <c r="H37" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="41">
+      <c r="A38" s="34">
         <v>305</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="36">
         <v>14.2</v>
       </c>
-      <c r="F38" s="27">
+      <c r="F38" s="25">
         <v>10.7</v>
       </c>
-      <c r="G38" s="27">
+      <c r="G38" s="25">
         <v>18.7</v>
       </c>
-      <c r="H38" s="44">
+      <c r="H38" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="41">
+      <c r="A39" s="34">
         <v>306</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="36">
         <v>6.3</v>
       </c>
-      <c r="F39" s="27">
+      <c r="F39" s="25">
         <v>3.8</v>
       </c>
-      <c r="G39" s="27">
+      <c r="G39" s="25">
         <v>10.3</v>
       </c>
-      <c r="H39" s="44">
+      <c r="H39" s="37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="41">
+      <c r="A40" s="34">
         <v>307</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="36">
         <v>11.5</v>
       </c>
       <c r="D40" t="s">
         <v>108</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="25">
         <v>8.1</v>
       </c>
-      <c r="G40" s="27">
+      <c r="G40" s="25">
         <v>15.9</v>
       </c>
-      <c r="H40" s="44">
+      <c r="H40" s="37">
         <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="41">
+      <c r="A41" s="34">
         <v>308</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="43">
+      <c r="C41" s="36">
         <v>12.7</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F41" s="25">
         <v>9.3000000000000007</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="25">
         <v>17</v>
       </c>
-      <c r="H41" s="44">
+      <c r="H41" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="41">
+      <c r="A42" s="34">
         <v>309</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="43">
+      <c r="C42" s="36">
         <v>14.8</v>
       </c>
-      <c r="F42" s="27">
+      <c r="F42" s="25">
         <v>11.2</v>
       </c>
-      <c r="G42" s="27">
+      <c r="G42" s="25">
         <v>19.3</v>
       </c>
-      <c r="H42" s="44">
+      <c r="H42" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="41">
+      <c r="A43" s="34">
         <v>310</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43" s="36">
         <v>10.8</v>
       </c>
-      <c r="F43" s="27">
+      <c r="F43" s="25">
         <v>7.4</v>
       </c>
-      <c r="G43" s="27">
+      <c r="G43" s="25">
         <v>15.5</v>
       </c>
-      <c r="H43" s="44">
+      <c r="H43" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="41">
+      <c r="A44" s="34">
         <v>311</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="36">
         <v>12.2</v>
       </c>
-      <c r="F44" s="27">
+      <c r="F44" s="25">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G44" s="27">
+      <c r="G44" s="25">
         <v>16.600000000000001</v>
       </c>
-      <c r="H44" s="44">
+      <c r="H44" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="41">
+      <c r="A45" s="34">
         <v>312</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="36">
         <v>9.4</v>
       </c>
-      <c r="F45" s="27">
+      <c r="F45" s="25">
         <v>6.5</v>
       </c>
-      <c r="G45" s="27">
+      <c r="G45" s="25">
         <v>13.3</v>
       </c>
-      <c r="H45" s="44">
+      <c r="H45" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="41">
+      <c r="A46" s="34">
         <v>313</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="36">
         <v>15</v>
       </c>
-      <c r="F46" s="27">
+      <c r="F46" s="25">
         <v>11.5</v>
       </c>
-      <c r="G46" s="27">
+      <c r="G46" s="25">
         <v>19.5</v>
       </c>
-      <c r="H46" s="44">
+      <c r="H46" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="41">
+      <c r="A47" s="34">
         <v>314</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="36">
         <v>12.9</v>
       </c>
-      <c r="F47" s="27">
+      <c r="F47" s="25">
         <v>9.1</v>
       </c>
-      <c r="G47" s="27">
+      <c r="G47" s="25">
         <v>17.899999999999999</v>
       </c>
-      <c r="H47" s="44">
+      <c r="H47" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="41">
+      <c r="A48" s="34">
         <v>315</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="36">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F48" s="27">
+      <c r="F48" s="25">
         <v>6.3</v>
       </c>
-      <c r="G48" s="27">
+      <c r="G48" s="25">
         <v>12.2</v>
       </c>
-      <c r="H48" s="44">
+      <c r="H48" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="41">
+      <c r="A49" s="34">
         <v>316</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="36">
         <v>13.5</v>
       </c>
       <c r="D49" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="27">
+      <c r="F49" s="25">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G49" s="27">
+      <c r="G49" s="25">
         <v>18.3</v>
       </c>
-      <c r="H49" s="44">
+      <c r="H49" s="37">
         <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="41">
+      <c r="A50" s="34">
         <v>317</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="36">
         <v>14.8</v>
       </c>
-      <c r="F50" s="27">
+      <c r="F50" s="25">
         <v>10.8</v>
       </c>
-      <c r="G50" s="27">
+      <c r="G50" s="25">
         <v>19.899999999999999</v>
       </c>
-      <c r="H50" s="44">
+      <c r="H50" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="41">
+      <c r="A51" s="34">
         <v>318</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="36">
         <v>13.9</v>
       </c>
-      <c r="F51" s="27">
+      <c r="F51" s="25">
         <v>10.199999999999999</v>
       </c>
-      <c r="G51" s="27">
+      <c r="G51" s="25">
         <v>18.8</v>
       </c>
-      <c r="H51" s="44">
+      <c r="H51" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="41">
+      <c r="A52" s="34">
         <v>401</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52" s="36">
         <v>11.2</v>
       </c>
-      <c r="F52" s="27">
+      <c r="F52" s="25">
         <v>8</v>
       </c>
-      <c r="G52" s="27">
+      <c r="G52" s="25">
         <v>15.4</v>
       </c>
-      <c r="H52" s="44">
+      <c r="H52" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="41">
+      <c r="A53" s="34">
         <v>402</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B53" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="43">
+      <c r="C53" s="36">
         <v>9.4</v>
       </c>
-      <c r="F53" s="27">
+      <c r="F53" s="25">
         <v>5.7</v>
       </c>
-      <c r="G53" s="27">
+      <c r="G53" s="25">
         <v>15.3</v>
       </c>
-      <c r="H53" s="44">
+      <c r="H53" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="41">
+      <c r="A54" s="34">
         <v>403</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B54" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="43">
+      <c r="C54" s="36">
         <v>13.4</v>
       </c>
-      <c r="F54" s="27">
+      <c r="F54" s="25">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G54" s="27">
+      <c r="G54" s="25">
         <v>19.2</v>
       </c>
-      <c r="H54" s="44">
+      <c r="H54" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="41">
+      <c r="A55" s="34">
         <v>404</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="36">
         <v>14.1</v>
       </c>
-      <c r="F55" s="27">
+      <c r="F55" s="25">
         <v>9.6</v>
       </c>
-      <c r="G55" s="27">
+      <c r="G55" s="25">
         <v>20.3</v>
       </c>
-      <c r="H55" s="44">
+      <c r="H55" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="41">
+      <c r="A56" s="34">
         <v>405</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="36">
         <v>7.5</v>
       </c>
       <c r="D56" t="s">
         <v>107</v>
       </c>
-      <c r="F56" s="27">
+      <c r="F56" s="25">
         <v>4.7</v>
       </c>
-      <c r="G56" s="27">
+      <c r="G56" s="25">
         <v>11.7</v>
       </c>
-      <c r="H56" s="44">
+      <c r="H56" s="37">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="41">
+      <c r="A57" s="34">
         <v>406</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="43">
+      <c r="C57" s="36">
         <v>6.8</v>
       </c>
-      <c r="F57" s="27">
+      <c r="F57" s="25">
         <v>4.7</v>
       </c>
-      <c r="G57" s="27">
+      <c r="G57" s="25">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H57" s="44">
+      <c r="H57" s="37">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="41">
+      <c r="A58" s="34">
         <v>407</v>
       </c>
-      <c r="B58" s="42" t="s">
+      <c r="B58" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C58" s="43">
+      <c r="C58" s="36">
         <v>8</v>
       </c>
-      <c r="F58" s="27">
+      <c r="F58" s="25">
         <v>5.3</v>
       </c>
-      <c r="G58" s="27">
+      <c r="G58" s="25">
         <v>12</v>
       </c>
-      <c r="H58" s="44">
+      <c r="H58" s="37">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="41">
+      <c r="A59" s="34">
         <v>408</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="B59" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="43">
+      <c r="C59" s="36">
         <v>14</v>
       </c>
-      <c r="F59" s="27">
+      <c r="F59" s="25">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G59" s="27">
+      <c r="G59" s="25">
         <v>19.600000000000001</v>
       </c>
-      <c r="H59" s="44">
+      <c r="H59" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="41">
+      <c r="A60" s="34">
         <v>409</v>
       </c>
-      <c r="B60" s="42" t="s">
+      <c r="B60" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="43">
+      <c r="C60" s="36">
         <v>14.5</v>
       </c>
       <c r="D60" t="s">
         <v>108</v>
       </c>
-      <c r="F60" s="27">
+      <c r="F60" s="25">
         <v>10.6</v>
       </c>
-      <c r="G60" s="27">
+      <c r="G60" s="25">
         <v>19.5</v>
       </c>
-      <c r="H60" s="44">
+      <c r="H60" s="37">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="41">
+      <c r="A61" s="34">
         <v>410</v>
       </c>
-      <c r="B61" s="42" t="s">
+      <c r="B61" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="43">
+      <c r="C61" s="36">
         <v>19.5</v>
       </c>
       <c r="D61" t="s">
         <v>108</v>
       </c>
-      <c r="F61" s="27">
+      <c r="F61" s="25">
         <v>14.4</v>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="25">
         <v>25.9</v>
       </c>
-      <c r="H61" s="44">
+      <c r="H61" s="37">
         <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="41">
+      <c r="A62" s="34">
         <v>411</v>
       </c>
-      <c r="B62" s="42" t="s">
+      <c r="B62" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="43">
+      <c r="C62" s="36">
         <v>7.2</v>
       </c>
-      <c r="F62" s="27">
+      <c r="F62" s="25">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G62" s="27">
+      <c r="G62" s="25">
         <v>10.3</v>
       </c>
-      <c r="H62" s="44">
+      <c r="H62" s="37">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="41">
+      <c r="A63" s="34">
         <v>412</v>
       </c>
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C63" s="43">
+      <c r="C63" s="36">
         <v>16.2</v>
       </c>
-      <c r="F63" s="27">
+      <c r="F63" s="25">
         <v>12.4</v>
       </c>
-      <c r="G63" s="27">
+      <c r="G63" s="25">
         <v>20.9</v>
       </c>
-      <c r="H63" s="44">
+      <c r="H63" s="37">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="41">
+      <c r="A64" s="34">
         <v>413</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="43">
+      <c r="C64" s="36">
         <v>14.5</v>
       </c>
       <c r="D64" t="s">
         <v>108</v>
       </c>
-      <c r="F64" s="27">
+      <c r="F64" s="25">
         <v>10.3</v>
       </c>
-      <c r="G64" s="27">
+      <c r="G64" s="25">
         <v>19.899999999999999</v>
       </c>
-      <c r="H64" s="44">
+      <c r="H64" s="37">
         <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="41">
+      <c r="A65" s="34">
         <v>414</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="43">
+      <c r="C65" s="36">
         <v>15</v>
       </c>
-      <c r="F65" s="27">
+      <c r="F65" s="25">
         <v>11.3</v>
       </c>
-      <c r="G65" s="27">
+      <c r="G65" s="25">
         <v>19.5</v>
       </c>
-      <c r="H65" s="44">
+      <c r="H65" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="41">
+      <c r="A66" s="34">
         <v>501</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C66" s="43">
+      <c r="C66" s="36">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F66" s="27">
+      <c r="F66" s="25">
         <v>6.8</v>
       </c>
-      <c r="G66" s="27">
+      <c r="G66" s="25">
         <v>12.6</v>
       </c>
-      <c r="H66" s="44">
+      <c r="H66" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="41">
+      <c r="A67" s="34">
         <v>502</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C67" s="43">
+      <c r="C67" s="36">
         <v>5.6</v>
       </c>
-      <c r="F67" s="27">
+      <c r="F67" s="25">
         <v>3.4</v>
       </c>
-      <c r="G67" s="27">
+      <c r="G67" s="25">
         <v>8.9</v>
       </c>
-      <c r="H67" s="44">
+      <c r="H67" s="37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="45">
+      <c r="A68" s="38">
         <v>503</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C68" s="47">
+      <c r="C68" s="40">
         <v>8.6</v>
       </c>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="49">
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="42">
         <v>6</v>
       </c>
-      <c r="G68" s="49">
+      <c r="G68" s="42">
         <v>12</v>
       </c>
-      <c r="H68" s="50">
+      <c r="H68" s="43">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="H69" s="27"/>
+      <c r="H69" s="25"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="H70" s="27"/>
+      <c r="H70" s="25"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="51" t="s">
+      <c r="A71" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="B71" s="52" t="s">
+      <c r="B71" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="C71" s="53" t="s">
+      <c r="C71" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54" t="s">
+      <c r="D71" s="47"/>
+      <c r="E71" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F71" s="53" t="s">
+      <c r="F71" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G71" s="40" t="s">
+      <c r="G71" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H71" s="55" t="s">
+      <c r="H71" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="41">
+      <c r="A72" s="34">
         <v>2</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C72" s="27">
+      <c r="C72" s="25">
         <v>16.2</v>
       </c>
-      <c r="F72" s="27">
+      <c r="F72" s="25">
         <v>14.7</v>
       </c>
-      <c r="G72" s="56">
+      <c r="G72" s="49">
         <v>17.7</v>
       </c>
-      <c r="H72" s="57">
+      <c r="H72" s="50">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="41">
+      <c r="A73" s="34">
         <v>3</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="C73" s="27">
+      <c r="C73" s="25">
         <v>11.9</v>
       </c>
-      <c r="F73" s="27">
+      <c r="F73" s="25">
         <v>11</v>
       </c>
-      <c r="G73" s="56">
+      <c r="G73" s="49">
         <v>12.9</v>
       </c>
-      <c r="H73" s="57">
+      <c r="H73" s="50">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="41">
+      <c r="A74" s="34">
         <v>1</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="27">
+      <c r="C74" s="25">
         <v>7.8</v>
       </c>
-      <c r="F74" s="27">
+      <c r="F74" s="25">
         <v>6.9</v>
       </c>
-      <c r="G74" s="56">
+      <c r="G74" s="49">
         <v>8.9</v>
       </c>
-      <c r="H74" s="57">
+      <c r="H74" s="50">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="41">
+      <c r="A75" s="34">
         <v>4</v>
       </c>
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C75" s="27">
+      <c r="C75" s="25">
         <v>11.3</v>
       </c>
-      <c r="F75" s="27">
+      <c r="F75" s="25">
         <v>10.199999999999999</v>
       </c>
-      <c r="G75" s="56">
+      <c r="G75" s="49">
         <v>12.5</v>
       </c>
-      <c r="H75" s="57">
+      <c r="H75" s="50">
         <f t="shared" ref="H75:H80" si="1">ROUND(C75,0)</f>
         <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="45">
+      <c r="A76" s="38">
         <v>5</v>
       </c>
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="49">
+      <c r="C76" s="42">
         <v>7.7</v>
       </c>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="49">
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
+      <c r="F76" s="42">
         <v>6.2</v>
       </c>
-      <c r="G76" s="58">
+      <c r="G76" s="51">
         <v>9.6</v>
       </c>
-      <c r="H76" s="59">
+      <c r="H76" s="52">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="H77" s="27"/>
+      <c r="H77" s="25"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="H78" s="27"/>
+      <c r="H78" s="25"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="B79" s="60" t="s">
+      <c r="B79" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C79" s="53" t="s">
+      <c r="C79" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D79" s="54"/>
-      <c r="E79" s="54" t="s">
+      <c r="D79" s="47"/>
+      <c r="E79" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F79" s="53" t="s">
+      <c r="F79" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G79" s="40" t="s">
+      <c r="G79" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H79" s="55" t="s">
+      <c r="H79" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:8">
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C80" s="61">
+      <c r="C80" s="54">
         <v>11.3</v>
       </c>
-      <c r="D80" s="62"/>
-      <c r="E80" s="62"/>
-      <c r="F80" s="61">
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="54">
         <v>10.8</v>
       </c>
-      <c r="G80" s="63">
+      <c r="G80" s="56">
         <v>11.9</v>
       </c>
-      <c r="H80" s="64">
+      <c r="H80" s="57">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -9029,1535 +9027,1535 @@
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="27" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="25" customWidth="1"/>
     <col min="4" max="4" width="3.33203125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="7" width="13.5" style="27" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="25" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="24" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="44.25" customHeight="1">
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="27" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54" t="s">
+      <c r="D9" s="47"/>
+      <c r="E9" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F9" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="33" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="41">
+      <c r="A10" s="34">
         <v>101</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="36">
         <v>91</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="25">
         <v>87.3</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="25">
         <v>93.6</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="59">
         <f>ROUND(C10,0)</f>
         <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="41">
+      <c r="A11" s="34">
         <v>102</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="36">
         <v>91</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="25">
         <v>87.3</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="25">
         <v>93.6</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="37">
         <f t="shared" ref="H11:H74" si="0">ROUND(C11,0)</f>
         <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="41">
+      <c r="A12" s="34">
         <v>103</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="36">
         <v>69.5</v>
       </c>
       <c r="D12" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="25">
         <v>63.7</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="25">
         <v>74.8</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="37">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="41">
+      <c r="A13" s="34">
         <v>104</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="36">
         <v>86.3</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="25">
         <v>81.5</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="25">
         <v>90</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="37">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="41">
+      <c r="A14" s="34">
         <v>105</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="36">
         <v>86.3</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="25">
         <v>81.5</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="25">
         <v>90</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="37">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="41">
+      <c r="A15" s="34">
         <v>106</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="36">
         <v>90.1</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="25">
         <v>85.3</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="25">
         <v>93.4</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="37">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="41">
+      <c r="A16" s="34">
         <v>107</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="36">
         <v>92.6</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="25">
         <v>88.5</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="25">
         <v>95.3</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="37">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="41">
+      <c r="A17" s="34">
         <v>108</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="36">
         <v>89.4</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="25">
         <v>83.6</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="25">
         <v>93.3</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="37">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="41">
+      <c r="A18" s="34">
         <v>109</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="36">
         <v>83.1</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="25">
         <v>77.599999999999994</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="25">
         <v>87.4</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="37">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="41">
+      <c r="A19" s="34">
         <v>110</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="36">
         <v>78.8</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="25">
         <v>73.3</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="25">
         <v>83.4</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="41">
+      <c r="A20" s="34">
         <v>111</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="36">
         <v>76.5</v>
       </c>
       <c r="D20" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="25">
         <v>70.3</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="25">
         <v>81.7</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="37">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="41">
+      <c r="A21" s="34">
         <v>112</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="36">
         <v>68.099999999999994</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="25">
         <v>61.6</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="25">
         <v>73.900000000000006</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="37">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="41">
+      <c r="A22" s="34">
         <v>201</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="36">
         <v>72</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="25">
         <v>64.900000000000006</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="25">
         <v>78.2</v>
       </c>
-      <c r="H22" s="44">
+      <c r="H22" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="41">
+      <c r="A23" s="34">
         <v>202</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="36">
         <v>72</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="25">
         <v>64.900000000000006</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="25">
         <v>78.2</v>
       </c>
-      <c r="H23" s="44">
+      <c r="H23" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="41">
+      <c r="A24" s="34">
         <v>203</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="36">
         <v>69.099999999999994</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="25">
         <v>63.5</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="25">
         <v>74.2</v>
       </c>
-      <c r="H24" s="44">
+      <c r="H24" s="37">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="41">
+      <c r="A25" s="34">
         <v>204</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="36">
         <v>72.099999999999994</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="25">
         <v>65.599999999999994</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="25">
         <v>77.8</v>
       </c>
-      <c r="H25" s="44">
+      <c r="H25" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="41">
+      <c r="A26" s="34">
         <v>205</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="36">
         <v>66.900000000000006</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="25">
         <v>60.4</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="25">
         <v>72.900000000000006</v>
       </c>
-      <c r="H26" s="44">
+      <c r="H26" s="37">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="41">
+      <c r="A27" s="34">
         <v>206</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="36">
         <v>69.099999999999994</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="25">
         <v>63.5</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="25">
         <v>74.2</v>
       </c>
-      <c r="H27" s="44">
+      <c r="H27" s="37">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="41">
+      <c r="A28" s="34">
         <v>207</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="36">
         <v>67.099999999999994</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="25">
         <v>60.8</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="25">
         <v>72.900000000000006</v>
       </c>
-      <c r="H28" s="44">
+      <c r="H28" s="37">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="41">
+      <c r="A29" s="34">
         <v>208</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="36">
         <v>82.7</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="25">
         <v>76.900000000000006</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="25">
         <v>87.3</v>
       </c>
-      <c r="H29" s="44">
+      <c r="H29" s="37">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="41">
+      <c r="A30" s="34">
         <v>209</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="36">
         <v>72</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="25">
         <v>66.2</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="25">
         <v>77.099999999999994</v>
       </c>
-      <c r="H30" s="44">
+      <c r="H30" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="41">
+      <c r="A31" s="34">
         <v>210</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="36">
         <v>76.599999999999994</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="25">
         <v>70.2</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="25">
         <v>81.900000000000006</v>
       </c>
-      <c r="H31" s="44">
+      <c r="H31" s="37">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="41">
+      <c r="A32" s="34">
         <v>211</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="36">
         <v>80.3</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="25">
         <v>74.5</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="25">
         <v>85.1</v>
       </c>
-      <c r="H32" s="44">
+      <c r="H32" s="37">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="41">
+      <c r="A33" s="34">
         <v>212</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="36">
         <v>77.900000000000006</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="25">
         <v>72.599999999999994</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="25">
         <v>82.4</v>
       </c>
-      <c r="H33" s="44">
+      <c r="H33" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="41">
+      <c r="A34" s="34">
         <v>301</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="36">
         <v>79.099999999999994</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="25">
         <v>73.8</v>
       </c>
-      <c r="G34" s="27">
+      <c r="G34" s="25">
         <v>83.5</v>
       </c>
-      <c r="H34" s="44">
+      <c r="H34" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="41">
+      <c r="A35" s="34">
         <v>302</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="36">
         <v>86.3</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="25">
         <v>80.900000000000006</v>
       </c>
-      <c r="G35" s="27">
+      <c r="G35" s="25">
         <v>90.3</v>
       </c>
-      <c r="H35" s="44">
+      <c r="H35" s="37">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="41">
+      <c r="A36" s="34">
         <v>303</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="36">
         <v>76</v>
       </c>
-      <c r="F36" s="27">
+      <c r="F36" s="25">
         <v>70.599999999999994</v>
       </c>
-      <c r="G36" s="27">
+      <c r="G36" s="25">
         <v>80.599999999999994</v>
       </c>
-      <c r="H36" s="44">
+      <c r="H36" s="37">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="41">
+      <c r="A37" s="34">
         <v>304</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="36">
         <v>71.400000000000006</v>
       </c>
-      <c r="F37" s="27">
+      <c r="F37" s="25">
         <v>64.3</v>
       </c>
-      <c r="G37" s="27">
+      <c r="G37" s="25">
         <v>77.5</v>
       </c>
-      <c r="H37" s="44">
+      <c r="H37" s="37">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="41">
+      <c r="A38" s="34">
         <v>305</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="36">
         <v>70.2</v>
       </c>
-      <c r="F38" s="27">
+      <c r="F38" s="25">
         <v>63.1</v>
       </c>
-      <c r="G38" s="27">
+      <c r="G38" s="25">
         <v>76.400000000000006</v>
       </c>
-      <c r="H38" s="44">
+      <c r="H38" s="37">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="41">
+      <c r="A39" s="34">
         <v>306</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="36">
         <v>88.4</v>
       </c>
-      <c r="F39" s="27">
+      <c r="F39" s="25">
         <v>83.8</v>
       </c>
-      <c r="G39" s="27">
+      <c r="G39" s="25">
         <v>91.8</v>
       </c>
-      <c r="H39" s="44">
+      <c r="H39" s="37">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="41">
+      <c r="A40" s="34">
         <v>307</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="36">
         <v>73.599999999999994</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="25">
         <v>67.400000000000006</v>
       </c>
-      <c r="G40" s="27">
+      <c r="G40" s="25">
         <v>79</v>
       </c>
-      <c r="H40" s="44">
+      <c r="H40" s="37">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="41">
+      <c r="A41" s="34">
         <v>308</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="43">
+      <c r="C41" s="36">
         <v>83.5</v>
       </c>
       <c r="D41" t="s">
         <v>107</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F41" s="25">
         <v>79</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="25">
         <v>87.2</v>
       </c>
-      <c r="H41" s="44">
+      <c r="H41" s="37">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="41">
+      <c r="A42" s="34">
         <v>309</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="43">
+      <c r="C42" s="36">
         <v>78</v>
       </c>
-      <c r="F42" s="27">
+      <c r="F42" s="25">
         <v>72.2</v>
       </c>
-      <c r="G42" s="27">
+      <c r="G42" s="25">
         <v>82.9</v>
       </c>
-      <c r="H42" s="44">
+      <c r="H42" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="41">
+      <c r="A43" s="34">
         <v>310</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43" s="36">
         <v>73.8</v>
       </c>
-      <c r="F43" s="27">
+      <c r="F43" s="25">
         <v>67.900000000000006</v>
       </c>
-      <c r="G43" s="27">
+      <c r="G43" s="25">
         <v>78.900000000000006</v>
       </c>
-      <c r="H43" s="44">
+      <c r="H43" s="37">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="41">
+      <c r="A44" s="34">
         <v>311</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="36">
         <v>65.400000000000006</v>
       </c>
-      <c r="F44" s="27">
+      <c r="F44" s="25">
         <v>59.6</v>
       </c>
-      <c r="G44" s="27">
+      <c r="G44" s="25">
         <v>70.7</v>
       </c>
-      <c r="H44" s="44">
+      <c r="H44" s="37">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="41">
+      <c r="A45" s="34">
         <v>312</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="36">
         <v>77.7</v>
       </c>
-      <c r="F45" s="27">
+      <c r="F45" s="25">
         <v>72.599999999999994</v>
       </c>
-      <c r="G45" s="27">
+      <c r="G45" s="25">
         <v>82.1</v>
       </c>
-      <c r="H45" s="44">
+      <c r="H45" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="41">
+      <c r="A46" s="34">
         <v>313</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="36">
         <v>69.7</v>
       </c>
-      <c r="F46" s="27">
+      <c r="F46" s="25">
         <v>63.6</v>
       </c>
-      <c r="G46" s="27">
+      <c r="G46" s="25">
         <v>75.099999999999994</v>
       </c>
-      <c r="H46" s="44">
+      <c r="H46" s="37">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="41">
+      <c r="A47" s="34">
         <v>314</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="36">
         <v>76.8</v>
       </c>
-      <c r="F47" s="27">
+      <c r="F47" s="25">
         <v>70.099999999999994</v>
       </c>
-      <c r="G47" s="27">
+      <c r="G47" s="25">
         <v>82.4</v>
       </c>
-      <c r="H47" s="44">
+      <c r="H47" s="37">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="41">
+      <c r="A48" s="34">
         <v>315</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="36">
         <v>69.900000000000006</v>
       </c>
-      <c r="F48" s="27">
+      <c r="F48" s="25">
         <v>64.400000000000006</v>
       </c>
-      <c r="G48" s="27">
+      <c r="G48" s="25">
         <v>74.900000000000006</v>
       </c>
-      <c r="H48" s="44">
+      <c r="H48" s="37">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="41">
+      <c r="A49" s="34">
         <v>316</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="36">
         <v>79.3</v>
       </c>
-      <c r="F49" s="27">
+      <c r="F49" s="25">
         <v>73.099999999999994</v>
       </c>
-      <c r="G49" s="27">
+      <c r="G49" s="25">
         <v>84.4</v>
       </c>
-      <c r="H49" s="44">
+      <c r="H49" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="41">
+      <c r="A50" s="34">
         <v>317</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="36">
         <v>83</v>
       </c>
-      <c r="F50" s="27">
+      <c r="F50" s="25">
         <v>77.400000000000006</v>
       </c>
-      <c r="G50" s="27">
+      <c r="G50" s="25">
         <v>87.5</v>
       </c>
-      <c r="H50" s="44">
+      <c r="H50" s="37">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="41">
+      <c r="A51" s="34">
         <v>318</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="36">
         <v>89.3</v>
       </c>
-      <c r="F51" s="27">
+      <c r="F51" s="25">
         <v>85.4</v>
       </c>
-      <c r="G51" s="27">
+      <c r="G51" s="25">
         <v>92.3</v>
       </c>
-      <c r="H51" s="44">
+      <c r="H51" s="37">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="41">
+      <c r="A52" s="34">
         <v>401</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52" s="36">
         <v>79.3</v>
       </c>
-      <c r="F52" s="27">
+      <c r="F52" s="25">
         <v>72.7</v>
       </c>
-      <c r="G52" s="27">
+      <c r="G52" s="25">
         <v>84.7</v>
       </c>
-      <c r="H52" s="44">
+      <c r="H52" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="41">
+      <c r="A53" s="34">
         <v>402</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B53" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="43">
+      <c r="C53" s="36">
         <v>79.099999999999994</v>
       </c>
-      <c r="F53" s="27">
+      <c r="F53" s="25">
         <v>72.599999999999994</v>
       </c>
-      <c r="G53" s="27">
+      <c r="G53" s="25">
         <v>84.4</v>
       </c>
-      <c r="H53" s="44">
+      <c r="H53" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="41">
+      <c r="A54" s="34">
         <v>403</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B54" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="43">
+      <c r="C54" s="36">
         <v>71.5</v>
       </c>
       <c r="D54" t="s">
         <v>107</v>
       </c>
-      <c r="F54" s="27">
+      <c r="F54" s="25">
         <v>65.599999999999994</v>
       </c>
-      <c r="G54" s="27">
+      <c r="G54" s="25">
         <v>76.7</v>
       </c>
-      <c r="H54" s="44">
+      <c r="H54" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="41">
+      <c r="A55" s="34">
         <v>404</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="36">
         <v>68.099999999999994</v>
       </c>
-      <c r="F55" s="27">
+      <c r="F55" s="25">
         <v>61.8</v>
       </c>
-      <c r="G55" s="27">
+      <c r="G55" s="25">
         <v>73.8</v>
       </c>
-      <c r="H55" s="44">
+      <c r="H55" s="37">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="41">
+      <c r="A56" s="34">
         <v>405</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="36">
         <v>78.400000000000006</v>
       </c>
-      <c r="F56" s="27">
+      <c r="F56" s="25">
         <v>71.7</v>
       </c>
-      <c r="G56" s="27">
+      <c r="G56" s="25">
         <v>83.9</v>
       </c>
-      <c r="H56" s="44">
+      <c r="H56" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="41">
+      <c r="A57" s="34">
         <v>406</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="43">
+      <c r="C57" s="36">
         <v>82</v>
       </c>
-      <c r="F57" s="27">
+      <c r="F57" s="25">
         <v>77.099999999999994</v>
       </c>
-      <c r="G57" s="27">
+      <c r="G57" s="25">
         <v>86</v>
       </c>
-      <c r="H57" s="44">
+      <c r="H57" s="37">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="41">
+      <c r="A58" s="34">
         <v>407</v>
       </c>
-      <c r="B58" s="42" t="s">
+      <c r="B58" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C58" s="43">
+      <c r="C58" s="36">
         <v>71.099999999999994</v>
       </c>
-      <c r="F58" s="27">
+      <c r="F58" s="25">
         <v>65.599999999999994</v>
       </c>
-      <c r="G58" s="27">
+      <c r="G58" s="25">
         <v>76.099999999999994</v>
       </c>
-      <c r="H58" s="44">
+      <c r="H58" s="37">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="41">
+      <c r="A59" s="34">
         <v>408</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="B59" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="43">
+      <c r="C59" s="36">
         <v>79.099999999999994</v>
       </c>
-      <c r="F59" s="27">
+      <c r="F59" s="25">
         <v>72.7</v>
       </c>
-      <c r="G59" s="27">
+      <c r="G59" s="25">
         <v>84.4</v>
       </c>
-      <c r="H59" s="44">
+      <c r="H59" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="41">
+      <c r="A60" s="34">
         <v>409</v>
       </c>
-      <c r="B60" s="42" t="s">
+      <c r="B60" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="43">
+      <c r="C60" s="36">
         <v>77.8</v>
       </c>
-      <c r="F60" s="27">
+      <c r="F60" s="25">
         <v>71.5</v>
       </c>
-      <c r="G60" s="27">
+      <c r="G60" s="25">
         <v>83.1</v>
       </c>
-      <c r="H60" s="44">
+      <c r="H60" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="41">
+      <c r="A61" s="34">
         <v>410</v>
       </c>
-      <c r="B61" s="42" t="s">
+      <c r="B61" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="43">
+      <c r="C61" s="36">
         <v>77</v>
       </c>
-      <c r="F61" s="27">
+      <c r="F61" s="25">
         <v>70.7</v>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="25">
         <v>82.3</v>
       </c>
-      <c r="H61" s="44">
+      <c r="H61" s="37">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="41">
+      <c r="A62" s="34">
         <v>411</v>
       </c>
-      <c r="B62" s="42" t="s">
+      <c r="B62" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="43">
+      <c r="C62" s="36">
         <v>85.7</v>
       </c>
-      <c r="F62" s="27">
+      <c r="F62" s="25">
         <v>81</v>
       </c>
-      <c r="G62" s="27">
+      <c r="G62" s="25">
         <v>89.4</v>
       </c>
-      <c r="H62" s="44">
+      <c r="H62" s="37">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="41">
+      <c r="A63" s="34">
         <v>412</v>
       </c>
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C63" s="43">
+      <c r="C63" s="36">
         <v>81.900000000000006</v>
       </c>
-      <c r="F63" s="27">
+      <c r="F63" s="25">
         <v>76.400000000000006</v>
       </c>
-      <c r="G63" s="27">
+      <c r="G63" s="25">
         <v>86.4</v>
       </c>
-      <c r="H63" s="44">
+      <c r="H63" s="37">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="41">
+      <c r="A64" s="34">
         <v>413</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="43">
+      <c r="C64" s="36">
         <v>74.400000000000006</v>
       </c>
-      <c r="F64" s="27">
+      <c r="F64" s="25">
         <v>66.3</v>
       </c>
-      <c r="G64" s="27">
+      <c r="G64" s="25">
         <v>81.099999999999994</v>
       </c>
-      <c r="H64" s="44">
+      <c r="H64" s="37">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="41">
+      <c r="A65" s="34">
         <v>414</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="43">
+      <c r="C65" s="36">
         <v>75.5</v>
       </c>
       <c r="D65" t="s">
         <v>108</v>
       </c>
-      <c r="F65" s="27">
+      <c r="F65" s="25">
         <v>69.2</v>
       </c>
-      <c r="G65" s="27">
+      <c r="G65" s="25">
         <v>80.8</v>
       </c>
-      <c r="H65" s="44">
+      <c r="H65" s="37">
         <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="41">
+      <c r="A66" s="34">
         <v>501</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C66" s="43">
+      <c r="C66" s="36">
         <v>77</v>
       </c>
-      <c r="F66" s="27">
+      <c r="F66" s="25">
         <v>70.2</v>
       </c>
-      <c r="G66" s="27">
+      <c r="G66" s="25">
         <v>82.7</v>
       </c>
-      <c r="H66" s="44">
+      <c r="H66" s="37">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="41">
+      <c r="A67" s="34">
         <v>502</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C67" s="43">
+      <c r="C67" s="36">
         <v>75.5</v>
       </c>
       <c r="D67" t="s">
         <v>107</v>
       </c>
-      <c r="F67" s="27">
+      <c r="F67" s="25">
         <v>66.3</v>
       </c>
-      <c r="G67" s="27">
+      <c r="G67" s="25">
         <v>82.9</v>
       </c>
-      <c r="H67" s="44">
+      <c r="H67" s="37">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="45">
+      <c r="A68" s="38">
         <v>503</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C68" s="47">
+      <c r="C68" s="40">
         <v>87.7</v>
       </c>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="49">
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="42">
         <v>82.9</v>
       </c>
-      <c r="G68" s="49">
+      <c r="G68" s="42">
         <v>91.3</v>
       </c>
-      <c r="H68" s="50">
+      <c r="H68" s="43">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="H69" s="27"/>
+      <c r="H69" s="25"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="H70" s="27"/>
+      <c r="H70" s="25"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="51" t="s">
+      <c r="A71" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="B71" s="52" t="s">
+      <c r="B71" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="C71" s="53" t="s">
+      <c r="C71" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54" t="s">
+      <c r="D71" s="47"/>
+      <c r="E71" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F71" s="53" t="s">
+      <c r="F71" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G71" s="40" t="s">
+      <c r="G71" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H71" s="55" t="s">
+      <c r="H71" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="41">
+      <c r="A72" s="34">
         <v>2</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C72" s="27">
+      <c r="C72" s="25">
         <v>73.400000000000006</v>
       </c>
-      <c r="F72" s="27">
+      <c r="F72" s="25">
         <v>71.400000000000006</v>
       </c>
-      <c r="G72" s="56">
+      <c r="G72" s="49">
         <v>75.3</v>
       </c>
-      <c r="H72" s="67">
+      <c r="H72" s="60">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="41">
+      <c r="A73" s="34">
         <v>3</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="C73" s="27">
+      <c r="C73" s="25">
         <v>76.900000000000006</v>
       </c>
-      <c r="F73" s="27">
+      <c r="F73" s="25">
         <v>75.599999999999994</v>
       </c>
-      <c r="G73" s="56">
+      <c r="G73" s="49">
         <v>78.2</v>
       </c>
-      <c r="H73" s="57">
+      <c r="H73" s="50">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="41">
+      <c r="A74" s="34">
         <v>1</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="27">
+      <c r="C74" s="25">
         <v>83.2</v>
       </c>
-      <c r="F74" s="27">
+      <c r="F74" s="25">
         <v>81.5</v>
       </c>
-      <c r="G74" s="56">
+      <c r="G74" s="49">
         <v>84.8</v>
       </c>
-      <c r="H74" s="57">
+      <c r="H74" s="50">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="41">
+      <c r="A75" s="34">
         <v>4</v>
       </c>
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C75" s="27">
+      <c r="C75" s="25">
         <v>76.400000000000006</v>
       </c>
-      <c r="F75" s="27">
+      <c r="F75" s="25">
         <v>74.7</v>
       </c>
-      <c r="G75" s="56">
+      <c r="G75" s="49">
         <v>78</v>
       </c>
-      <c r="H75" s="57">
+      <c r="H75" s="50">
         <f t="shared" ref="H75:H80" si="1">ROUND(C75,0)</f>
         <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="45">
+      <c r="A76" s="38">
         <v>5</v>
       </c>
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="49">
+      <c r="C76" s="42">
         <v>81.099999999999994</v>
       </c>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="49">
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
+      <c r="F76" s="42">
         <v>77.400000000000006</v>
       </c>
-      <c r="G76" s="58">
+      <c r="G76" s="51">
         <v>84.4</v>
       </c>
-      <c r="H76" s="59">
+      <c r="H76" s="52">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="H77" s="27"/>
+      <c r="H77" s="25"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="H78" s="27"/>
+      <c r="H78" s="25"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="B79" s="60" t="s">
+      <c r="B79" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C79" s="53" t="s">
+      <c r="C79" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D79" s="54"/>
-      <c r="E79" s="54" t="s">
+      <c r="D79" s="47"/>
+      <c r="E79" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F79" s="53" t="s">
+      <c r="F79" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G79" s="40" t="s">
+      <c r="G79" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H79" s="55" t="s">
+      <c r="H79" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:8">
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C80" s="61">
+      <c r="C80" s="54">
         <v>77.8</v>
       </c>
-      <c r="D80" s="62"/>
-      <c r="E80" s="62"/>
-      <c r="F80" s="61">
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="54">
         <v>77</v>
       </c>
-      <c r="G80" s="63">
+      <c r="G80" s="56">
         <v>78.599999999999994</v>
       </c>
-      <c r="H80" s="64">
+      <c r="H80" s="57">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
@@ -10795,6 +10793,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="4eab1d2f-0a6f-43b5-bd47-0cc182e7f81d" xsi:nil="true"/>
@@ -10803,15 +10810,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10834,6 +10832,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6697668-EC76-46C6-A886-FE46F18A5C65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBDC9F0A-70B2-4955-92FB-558444EE0082}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10842,12 +10848,4 @@
     <ds:schemaRef ds:uri="18262a4b-7b39-4d27-b1ee-8cb22edac4a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6697668-EC76-46C6-A886-FE46F18A5C65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ingest new transportation data for 2023 update (#319)
* add test for ingestion helpers

* add ingest_helpers.py

* add ingest files to test triggers

* latest health excel file

* don't need R in dev container

* use read_excel helper in health script

* fix file

* change name of dict with column mappings

* drop todo note

* use local file instead of s3

* process new transportation data

* add transportation data

* less printing

* better names for tests

* write metadata when reading from excel
</commit_message>
<xml_diff>
--- a/resources/quality_of_life/diabetes_self_report/diabetes_self_report_processed_2023.xlsx
+++ b/resources/quality_of_life/diabetes_self_report/diabetes_self_report_processed_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damonmccullough/github/db-equitable-development-tool/resources/quality_of_life/diabetes_self_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3B90C7-D265-0443-8968-10766D1B1DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A44FAC-5B22-6040-BD49-2BC7F0312B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32120" yWindow="-3100" windowWidth="29040" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31900" yWindow="-3100" windowWidth="29040" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCHP_Diabetes_SelfRepHealth" sheetId="6" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -670,7 +670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -719,12 +719,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -739,21 +733,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -811,6 +790,30 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12"/>
@@ -4230,28 +4233,23 @@
       <c r="A67" s="1"/>
     </row>
     <row r="69" spans="1:15" ht="25.5" customHeight="1">
-      <c r="A69" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-      <c r="L69" s="18"/>
-      <c r="M69" s="18"/>
-      <c r="N69" s="18"/>
-      <c r="O69" s="18"/>
+      <c r="A69" s="68"/>
+      <c r="B69" s="68"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="68"/>
+      <c r="H69" s="68"/>
+      <c r="I69" s="68"/>
+      <c r="J69" s="68"/>
+      <c r="K69" s="68"/>
+      <c r="L69" s="68"/>
+      <c r="M69" s="68"/>
+      <c r="N69" s="68"/>
+      <c r="O69" s="68"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A69:O69"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4286,26 +4284,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="35.25" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7430,23 +7428,23 @@
       <c r="A73" s="1"/>
     </row>
     <row r="75" spans="1:15" ht="25.5" customHeight="1">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="18"/>
-      <c r="L75" s="18"/>
-      <c r="M75" s="18"/>
-      <c r="N75" s="18"/>
-      <c r="O75" s="18"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="61"/>
+      <c r="G75" s="61"/>
+      <c r="H75" s="61"/>
+      <c r="I75" s="61"/>
+      <c r="J75" s="61"/>
+      <c r="K75" s="61"/>
+      <c r="L75" s="61"/>
+      <c r="M75" s="61"/>
+      <c r="N75" s="61"/>
+      <c r="O75" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7461,7 +7459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06904A75-F3E9-5846-B1B7-7F6541B0232E}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -7469,1541 +7467,1541 @@
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="27" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="25" customWidth="1"/>
     <col min="4" max="4" width="3.33203125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="7" width="13.5" style="27" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="25" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="24" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="30.75" customHeight="1">
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="27" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="33" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="41">
+      <c r="A10" s="34">
         <v>101</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="36">
         <v>3.4</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="25">
         <v>1.9</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="25">
         <v>6</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="37">
         <f>ROUND(C10,0)</f>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="41">
+      <c r="A11" s="34">
         <v>102</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="36">
         <v>3.4</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="25">
         <v>1.9</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="25">
         <v>6</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="37">
         <f t="shared" ref="H11:H74" si="0">ROUND(C11,0)</f>
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="41">
+      <c r="A12" s="34">
         <v>103</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="36">
         <v>10.7</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="25">
         <v>7.7</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="25">
         <v>14.8</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="41">
+      <c r="A13" s="34">
         <v>104</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="36">
         <v>5</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="25">
         <v>3.2</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="25">
         <v>7.8</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="37">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="41">
+      <c r="A14" s="34">
         <v>105</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="36">
         <v>5</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="25">
         <v>3.2</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="25">
         <v>7.8</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="37">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="41">
+      <c r="A15" s="34">
         <v>106</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="36">
         <v>4</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="25">
         <v>2.4</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="25">
         <v>6.3</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="37">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="41">
+      <c r="A16" s="34">
         <v>107</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="36">
         <v>5.3</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="25">
         <v>3.1</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="25">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="37">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="41">
+      <c r="A17" s="34">
         <v>108</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="36">
         <v>3.6</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="25">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="25">
         <v>5.9</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="37">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="41">
+      <c r="A18" s="34">
         <v>109</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="36">
         <v>9.6</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="25">
         <v>6.7</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="25">
         <v>13.5</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="37">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="41">
+      <c r="A19" s="34">
         <v>110</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="36">
         <v>12.2</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="25">
         <v>9</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="25">
         <v>16.2</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="41">
+      <c r="A20" s="34">
         <v>111</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="36">
         <v>16.5</v>
       </c>
       <c r="D20" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="25">
         <v>12.5</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="25">
         <v>21.6</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="37">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="41">
+      <c r="A21" s="34">
         <v>112</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="36">
         <v>12.9</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="25">
         <v>9.6</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="25">
         <v>17.100000000000001</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="41">
+      <c r="A22" s="34">
         <v>201</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="36">
         <v>20.399999999999999</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="25">
         <v>15.4</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="25">
         <v>26.6</v>
       </c>
-      <c r="H22" s="44">
+      <c r="H22" s="37">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="41">
+      <c r="A23" s="34">
         <v>202</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="36">
         <v>20.399999999999999</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="25">
         <v>15.4</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="25">
         <v>26.6</v>
       </c>
-      <c r="H23" s="44">
+      <c r="H23" s="37">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="41">
+      <c r="A24" s="34">
         <v>203</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="36">
         <v>22</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="25">
         <v>17.8</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="25">
         <v>26.9</v>
       </c>
-      <c r="H24" s="44">
+      <c r="H24" s="37">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="41">
+      <c r="A25" s="34">
         <v>204</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="36">
         <v>16.899999999999999</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="25">
         <v>12.6</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="25">
         <v>22.4</v>
       </c>
-      <c r="H25" s="44">
+      <c r="H25" s="37">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="41">
+      <c r="A26" s="34">
         <v>205</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="36">
         <v>15.8</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="25">
         <v>11.7</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="25">
         <v>21.1</v>
       </c>
-      <c r="H26" s="44">
+      <c r="H26" s="37">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="41">
+      <c r="A27" s="34">
         <v>206</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="36">
         <v>22</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="25">
         <v>17.8</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="25">
         <v>26.9</v>
       </c>
-      <c r="H27" s="44">
+      <c r="H27" s="37">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="41">
+      <c r="A28" s="34">
         <v>207</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="36">
         <v>18.5</v>
       </c>
       <c r="D28" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="25">
         <v>14.3</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="25">
         <v>23.7</v>
       </c>
-      <c r="H28" s="44">
+      <c r="H28" s="37">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="41">
+      <c r="A29" s="34">
         <v>208</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="36">
         <v>12.3</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="25">
         <v>7.3</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="25">
         <v>19.899999999999999</v>
       </c>
-      <c r="H29" s="44">
+      <c r="H29" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="41">
+      <c r="A30" s="34">
         <v>209</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="36">
         <v>15.6</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="25">
         <v>11.8</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="25">
         <v>20.5</v>
       </c>
-      <c r="H30" s="44">
+      <c r="H30" s="37">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="41">
+      <c r="A31" s="34">
         <v>210</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="36">
         <v>13.4</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="25">
         <v>10</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="25">
         <v>17.899999999999999</v>
       </c>
-      <c r="H31" s="44">
+      <c r="H31" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="41">
+      <c r="A32" s="34">
         <v>211</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="36">
         <v>13.5</v>
       </c>
       <c r="D32" t="s">
         <v>107</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="25">
         <v>9.9</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="25">
         <v>18.2</v>
       </c>
-      <c r="H32" s="44">
+      <c r="H32" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="41">
+      <c r="A33" s="34">
         <v>212</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="36">
         <v>14.1</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="25">
         <v>10.7</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="25">
         <v>18.3</v>
       </c>
-      <c r="H33" s="44">
+      <c r="H33" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="41">
+      <c r="A34" s="34">
         <v>301</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="36">
         <v>11.1</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="25">
         <v>7.8</v>
       </c>
-      <c r="G34" s="27">
+      <c r="G34" s="25">
         <v>15.7</v>
       </c>
-      <c r="H34" s="44">
+      <c r="H34" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="41">
+      <c r="A35" s="34">
         <v>302</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="36">
         <v>6</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="25">
         <v>3.6</v>
       </c>
-      <c r="G35" s="27">
+      <c r="G35" s="25">
         <v>9.9</v>
       </c>
-      <c r="H35" s="44">
+      <c r="H35" s="37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="41">
+      <c r="A36" s="34">
         <v>303</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="36">
         <v>13.2</v>
       </c>
-      <c r="F36" s="27">
+      <c r="F36" s="25">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G36" s="27">
+      <c r="G36" s="25">
         <v>17.8</v>
       </c>
-      <c r="H36" s="44">
+      <c r="H36" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="41">
+      <c r="A37" s="34">
         <v>304</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="36">
         <v>13.1</v>
       </c>
-      <c r="F37" s="27">
+      <c r="F37" s="25">
         <v>9.5</v>
       </c>
-      <c r="G37" s="27">
+      <c r="G37" s="25">
         <v>17.8</v>
       </c>
-      <c r="H37" s="44">
+      <c r="H37" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="41">
+      <c r="A38" s="34">
         <v>305</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="36">
         <v>14.2</v>
       </c>
-      <c r="F38" s="27">
+      <c r="F38" s="25">
         <v>10.7</v>
       </c>
-      <c r="G38" s="27">
+      <c r="G38" s="25">
         <v>18.7</v>
       </c>
-      <c r="H38" s="44">
+      <c r="H38" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="41">
+      <c r="A39" s="34">
         <v>306</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="36">
         <v>6.3</v>
       </c>
-      <c r="F39" s="27">
+      <c r="F39" s="25">
         <v>3.8</v>
       </c>
-      <c r="G39" s="27">
+      <c r="G39" s="25">
         <v>10.3</v>
       </c>
-      <c r="H39" s="44">
+      <c r="H39" s="37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="41">
+      <c r="A40" s="34">
         <v>307</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="36">
         <v>11.5</v>
       </c>
       <c r="D40" t="s">
         <v>108</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="25">
         <v>8.1</v>
       </c>
-      <c r="G40" s="27">
+      <c r="G40" s="25">
         <v>15.9</v>
       </c>
-      <c r="H40" s="44">
+      <c r="H40" s="37">
         <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="41">
+      <c r="A41" s="34">
         <v>308</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="43">
+      <c r="C41" s="36">
         <v>12.7</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F41" s="25">
         <v>9.3000000000000007</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="25">
         <v>17</v>
       </c>
-      <c r="H41" s="44">
+      <c r="H41" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="41">
+      <c r="A42" s="34">
         <v>309</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="43">
+      <c r="C42" s="36">
         <v>14.8</v>
       </c>
-      <c r="F42" s="27">
+      <c r="F42" s="25">
         <v>11.2</v>
       </c>
-      <c r="G42" s="27">
+      <c r="G42" s="25">
         <v>19.3</v>
       </c>
-      <c r="H42" s="44">
+      <c r="H42" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="41">
+      <c r="A43" s="34">
         <v>310</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43" s="36">
         <v>10.8</v>
       </c>
-      <c r="F43" s="27">
+      <c r="F43" s="25">
         <v>7.4</v>
       </c>
-      <c r="G43" s="27">
+      <c r="G43" s="25">
         <v>15.5</v>
       </c>
-      <c r="H43" s="44">
+      <c r="H43" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="41">
+      <c r="A44" s="34">
         <v>311</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="36">
         <v>12.2</v>
       </c>
-      <c r="F44" s="27">
+      <c r="F44" s="25">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G44" s="27">
+      <c r="G44" s="25">
         <v>16.600000000000001</v>
       </c>
-      <c r="H44" s="44">
+      <c r="H44" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="41">
+      <c r="A45" s="34">
         <v>312</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="36">
         <v>9.4</v>
       </c>
-      <c r="F45" s="27">
+      <c r="F45" s="25">
         <v>6.5</v>
       </c>
-      <c r="G45" s="27">
+      <c r="G45" s="25">
         <v>13.3</v>
       </c>
-      <c r="H45" s="44">
+      <c r="H45" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="41">
+      <c r="A46" s="34">
         <v>313</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="36">
         <v>15</v>
       </c>
-      <c r="F46" s="27">
+      <c r="F46" s="25">
         <v>11.5</v>
       </c>
-      <c r="G46" s="27">
+      <c r="G46" s="25">
         <v>19.5</v>
       </c>
-      <c r="H46" s="44">
+      <c r="H46" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="41">
+      <c r="A47" s="34">
         <v>314</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="36">
         <v>12.9</v>
       </c>
-      <c r="F47" s="27">
+      <c r="F47" s="25">
         <v>9.1</v>
       </c>
-      <c r="G47" s="27">
+      <c r="G47" s="25">
         <v>17.899999999999999</v>
       </c>
-      <c r="H47" s="44">
+      <c r="H47" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="41">
+      <c r="A48" s="34">
         <v>315</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="36">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F48" s="27">
+      <c r="F48" s="25">
         <v>6.3</v>
       </c>
-      <c r="G48" s="27">
+      <c r="G48" s="25">
         <v>12.2</v>
       </c>
-      <c r="H48" s="44">
+      <c r="H48" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="41">
+      <c r="A49" s="34">
         <v>316</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="36">
         <v>13.5</v>
       </c>
       <c r="D49" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="27">
+      <c r="F49" s="25">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G49" s="27">
+      <c r="G49" s="25">
         <v>18.3</v>
       </c>
-      <c r="H49" s="44">
+      <c r="H49" s="37">
         <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="41">
+      <c r="A50" s="34">
         <v>317</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="36">
         <v>14.8</v>
       </c>
-      <c r="F50" s="27">
+      <c r="F50" s="25">
         <v>10.8</v>
       </c>
-      <c r="G50" s="27">
+      <c r="G50" s="25">
         <v>19.899999999999999</v>
       </c>
-      <c r="H50" s="44">
+      <c r="H50" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="41">
+      <c r="A51" s="34">
         <v>318</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="36">
         <v>13.9</v>
       </c>
-      <c r="F51" s="27">
+      <c r="F51" s="25">
         <v>10.199999999999999</v>
       </c>
-      <c r="G51" s="27">
+      <c r="G51" s="25">
         <v>18.8</v>
       </c>
-      <c r="H51" s="44">
+      <c r="H51" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="41">
+      <c r="A52" s="34">
         <v>401</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52" s="36">
         <v>11.2</v>
       </c>
-      <c r="F52" s="27">
+      <c r="F52" s="25">
         <v>8</v>
       </c>
-      <c r="G52" s="27">
+      <c r="G52" s="25">
         <v>15.4</v>
       </c>
-      <c r="H52" s="44">
+      <c r="H52" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="41">
+      <c r="A53" s="34">
         <v>402</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B53" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="43">
+      <c r="C53" s="36">
         <v>9.4</v>
       </c>
-      <c r="F53" s="27">
+      <c r="F53" s="25">
         <v>5.7</v>
       </c>
-      <c r="G53" s="27">
+      <c r="G53" s="25">
         <v>15.3</v>
       </c>
-      <c r="H53" s="44">
+      <c r="H53" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="41">
+      <c r="A54" s="34">
         <v>403</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B54" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="43">
+      <c r="C54" s="36">
         <v>13.4</v>
       </c>
-      <c r="F54" s="27">
+      <c r="F54" s="25">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G54" s="27">
+      <c r="G54" s="25">
         <v>19.2</v>
       </c>
-      <c r="H54" s="44">
+      <c r="H54" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="41">
+      <c r="A55" s="34">
         <v>404</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="36">
         <v>14.1</v>
       </c>
-      <c r="F55" s="27">
+      <c r="F55" s="25">
         <v>9.6</v>
       </c>
-      <c r="G55" s="27">
+      <c r="G55" s="25">
         <v>20.3</v>
       </c>
-      <c r="H55" s="44">
+      <c r="H55" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="41">
+      <c r="A56" s="34">
         <v>405</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="36">
         <v>7.5</v>
       </c>
       <c r="D56" t="s">
         <v>107</v>
       </c>
-      <c r="F56" s="27">
+      <c r="F56" s="25">
         <v>4.7</v>
       </c>
-      <c r="G56" s="27">
+      <c r="G56" s="25">
         <v>11.7</v>
       </c>
-      <c r="H56" s="44">
+      <c r="H56" s="37">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="41">
+      <c r="A57" s="34">
         <v>406</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="43">
+      <c r="C57" s="36">
         <v>6.8</v>
       </c>
-      <c r="F57" s="27">
+      <c r="F57" s="25">
         <v>4.7</v>
       </c>
-      <c r="G57" s="27">
+      <c r="G57" s="25">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H57" s="44">
+      <c r="H57" s="37">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="41">
+      <c r="A58" s="34">
         <v>407</v>
       </c>
-      <c r="B58" s="42" t="s">
+      <c r="B58" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C58" s="43">
+      <c r="C58" s="36">
         <v>8</v>
       </c>
-      <c r="F58" s="27">
+      <c r="F58" s="25">
         <v>5.3</v>
       </c>
-      <c r="G58" s="27">
+      <c r="G58" s="25">
         <v>12</v>
       </c>
-      <c r="H58" s="44">
+      <c r="H58" s="37">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="41">
+      <c r="A59" s="34">
         <v>408</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="B59" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="43">
+      <c r="C59" s="36">
         <v>14</v>
       </c>
-      <c r="F59" s="27">
+      <c r="F59" s="25">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G59" s="27">
+      <c r="G59" s="25">
         <v>19.600000000000001</v>
       </c>
-      <c r="H59" s="44">
+      <c r="H59" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="41">
+      <c r="A60" s="34">
         <v>409</v>
       </c>
-      <c r="B60" s="42" t="s">
+      <c r="B60" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="43">
+      <c r="C60" s="36">
         <v>14.5</v>
       </c>
       <c r="D60" t="s">
         <v>108</v>
       </c>
-      <c r="F60" s="27">
+      <c r="F60" s="25">
         <v>10.6</v>
       </c>
-      <c r="G60" s="27">
+      <c r="G60" s="25">
         <v>19.5</v>
       </c>
-      <c r="H60" s="44">
+      <c r="H60" s="37">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="41">
+      <c r="A61" s="34">
         <v>410</v>
       </c>
-      <c r="B61" s="42" t="s">
+      <c r="B61" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="43">
+      <c r="C61" s="36">
         <v>19.5</v>
       </c>
       <c r="D61" t="s">
         <v>108</v>
       </c>
-      <c r="F61" s="27">
+      <c r="F61" s="25">
         <v>14.4</v>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="25">
         <v>25.9</v>
       </c>
-      <c r="H61" s="44">
+      <c r="H61" s="37">
         <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="41">
+      <c r="A62" s="34">
         <v>411</v>
       </c>
-      <c r="B62" s="42" t="s">
+      <c r="B62" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="43">
+      <c r="C62" s="36">
         <v>7.2</v>
       </c>
-      <c r="F62" s="27">
+      <c r="F62" s="25">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G62" s="27">
+      <c r="G62" s="25">
         <v>10.3</v>
       </c>
-      <c r="H62" s="44">
+      <c r="H62" s="37">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="41">
+      <c r="A63" s="34">
         <v>412</v>
       </c>
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C63" s="43">
+      <c r="C63" s="36">
         <v>16.2</v>
       </c>
-      <c r="F63" s="27">
+      <c r="F63" s="25">
         <v>12.4</v>
       </c>
-      <c r="G63" s="27">
+      <c r="G63" s="25">
         <v>20.9</v>
       </c>
-      <c r="H63" s="44">
+      <c r="H63" s="37">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="41">
+      <c r="A64" s="34">
         <v>413</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="43">
+      <c r="C64" s="36">
         <v>14.5</v>
       </c>
       <c r="D64" t="s">
         <v>108</v>
       </c>
-      <c r="F64" s="27">
+      <c r="F64" s="25">
         <v>10.3</v>
       </c>
-      <c r="G64" s="27">
+      <c r="G64" s="25">
         <v>19.899999999999999</v>
       </c>
-      <c r="H64" s="44">
+      <c r="H64" s="37">
         <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="41">
+      <c r="A65" s="34">
         <v>414</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="43">
+      <c r="C65" s="36">
         <v>15</v>
       </c>
-      <c r="F65" s="27">
+      <c r="F65" s="25">
         <v>11.3</v>
       </c>
-      <c r="G65" s="27">
+      <c r="G65" s="25">
         <v>19.5</v>
       </c>
-      <c r="H65" s="44">
+      <c r="H65" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="41">
+      <c r="A66" s="34">
         <v>501</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C66" s="43">
+      <c r="C66" s="36">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F66" s="27">
+      <c r="F66" s="25">
         <v>6.8</v>
       </c>
-      <c r="G66" s="27">
+      <c r="G66" s="25">
         <v>12.6</v>
       </c>
-      <c r="H66" s="44">
+      <c r="H66" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="41">
+      <c r="A67" s="34">
         <v>502</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C67" s="43">
+      <c r="C67" s="36">
         <v>5.6</v>
       </c>
-      <c r="F67" s="27">
+      <c r="F67" s="25">
         <v>3.4</v>
       </c>
-      <c r="G67" s="27">
+      <c r="G67" s="25">
         <v>8.9</v>
       </c>
-      <c r="H67" s="44">
+      <c r="H67" s="37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="45">
+      <c r="A68" s="38">
         <v>503</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C68" s="47">
+      <c r="C68" s="40">
         <v>8.6</v>
       </c>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="49">
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="42">
         <v>6</v>
       </c>
-      <c r="G68" s="49">
+      <c r="G68" s="42">
         <v>12</v>
       </c>
-      <c r="H68" s="50">
+      <c r="H68" s="43">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="H69" s="27"/>
+      <c r="H69" s="25"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="H70" s="27"/>
+      <c r="H70" s="25"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="51" t="s">
+      <c r="A71" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="B71" s="52" t="s">
+      <c r="B71" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="C71" s="53" t="s">
+      <c r="C71" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54" t="s">
+      <c r="D71" s="47"/>
+      <c r="E71" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F71" s="53" t="s">
+      <c r="F71" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G71" s="40" t="s">
+      <c r="G71" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H71" s="55" t="s">
+      <c r="H71" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="41">
+      <c r="A72" s="34">
         <v>2</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C72" s="27">
+      <c r="C72" s="25">
         <v>16.2</v>
       </c>
-      <c r="F72" s="27">
+      <c r="F72" s="25">
         <v>14.7</v>
       </c>
-      <c r="G72" s="56">
+      <c r="G72" s="49">
         <v>17.7</v>
       </c>
-      <c r="H72" s="57">
+      <c r="H72" s="50">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="41">
+      <c r="A73" s="34">
         <v>3</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="C73" s="27">
+      <c r="C73" s="25">
         <v>11.9</v>
       </c>
-      <c r="F73" s="27">
+      <c r="F73" s="25">
         <v>11</v>
       </c>
-      <c r="G73" s="56">
+      <c r="G73" s="49">
         <v>12.9</v>
       </c>
-      <c r="H73" s="57">
+      <c r="H73" s="50">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="41">
+      <c r="A74" s="34">
         <v>1</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="27">
+      <c r="C74" s="25">
         <v>7.8</v>
       </c>
-      <c r="F74" s="27">
+      <c r="F74" s="25">
         <v>6.9</v>
       </c>
-      <c r="G74" s="56">
+      <c r="G74" s="49">
         <v>8.9</v>
       </c>
-      <c r="H74" s="57">
+      <c r="H74" s="50">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="41">
+      <c r="A75" s="34">
         <v>4</v>
       </c>
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C75" s="27">
+      <c r="C75" s="25">
         <v>11.3</v>
       </c>
-      <c r="F75" s="27">
+      <c r="F75" s="25">
         <v>10.199999999999999</v>
       </c>
-      <c r="G75" s="56">
+      <c r="G75" s="49">
         <v>12.5</v>
       </c>
-      <c r="H75" s="57">
+      <c r="H75" s="50">
         <f t="shared" ref="H75:H80" si="1">ROUND(C75,0)</f>
         <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="45">
+      <c r="A76" s="38">
         <v>5</v>
       </c>
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="49">
+      <c r="C76" s="42">
         <v>7.7</v>
       </c>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="49">
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
+      <c r="F76" s="42">
         <v>6.2</v>
       </c>
-      <c r="G76" s="58">
+      <c r="G76" s="51">
         <v>9.6</v>
       </c>
-      <c r="H76" s="59">
+      <c r="H76" s="52">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="H77" s="27"/>
+      <c r="H77" s="25"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="H78" s="27"/>
+      <c r="H78" s="25"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="B79" s="60" t="s">
+      <c r="B79" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C79" s="53" t="s">
+      <c r="C79" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D79" s="54"/>
-      <c r="E79" s="54" t="s">
+      <c r="D79" s="47"/>
+      <c r="E79" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F79" s="53" t="s">
+      <c r="F79" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G79" s="40" t="s">
+      <c r="G79" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H79" s="55" t="s">
+      <c r="H79" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:8">
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C80" s="61">
+      <c r="C80" s="54">
         <v>11.3</v>
       </c>
-      <c r="D80" s="62"/>
-      <c r="E80" s="62"/>
-      <c r="F80" s="61">
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="54">
         <v>10.8</v>
       </c>
-      <c r="G80" s="63">
+      <c r="G80" s="56">
         <v>11.9</v>
       </c>
-      <c r="H80" s="64">
+      <c r="H80" s="57">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -9029,1535 +9027,1535 @@
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="27" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="25" customWidth="1"/>
     <col min="4" max="4" width="3.33203125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="7" width="13.5" style="27" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="25" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="24" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="44.25" customHeight="1">
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="27" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54" t="s">
+      <c r="D9" s="47"/>
+      <c r="E9" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F9" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="33" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="41">
+      <c r="A10" s="34">
         <v>101</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="36">
         <v>91</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="25">
         <v>87.3</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="25">
         <v>93.6</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="59">
         <f>ROUND(C10,0)</f>
         <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="41">
+      <c r="A11" s="34">
         <v>102</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="36">
         <v>91</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="25">
         <v>87.3</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="25">
         <v>93.6</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="37">
         <f t="shared" ref="H11:H74" si="0">ROUND(C11,0)</f>
         <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="41">
+      <c r="A12" s="34">
         <v>103</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="36">
         <v>69.5</v>
       </c>
       <c r="D12" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="25">
         <v>63.7</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="25">
         <v>74.8</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="37">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="41">
+      <c r="A13" s="34">
         <v>104</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="36">
         <v>86.3</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="25">
         <v>81.5</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="25">
         <v>90</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="37">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="41">
+      <c r="A14" s="34">
         <v>105</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="36">
         <v>86.3</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="25">
         <v>81.5</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="25">
         <v>90</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="37">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="41">
+      <c r="A15" s="34">
         <v>106</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="36">
         <v>90.1</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="25">
         <v>85.3</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="25">
         <v>93.4</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="37">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="41">
+      <c r="A16" s="34">
         <v>107</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="36">
         <v>92.6</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="25">
         <v>88.5</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="25">
         <v>95.3</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="37">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="41">
+      <c r="A17" s="34">
         <v>108</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="36">
         <v>89.4</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="25">
         <v>83.6</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="25">
         <v>93.3</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="37">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="41">
+      <c r="A18" s="34">
         <v>109</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="36">
         <v>83.1</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="25">
         <v>77.599999999999994</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="25">
         <v>87.4</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="37">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="41">
+      <c r="A19" s="34">
         <v>110</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="36">
         <v>78.8</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="25">
         <v>73.3</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="25">
         <v>83.4</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="41">
+      <c r="A20" s="34">
         <v>111</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="36">
         <v>76.5</v>
       </c>
       <c r="D20" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="25">
         <v>70.3</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="25">
         <v>81.7</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="37">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="41">
+      <c r="A21" s="34">
         <v>112</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="36">
         <v>68.099999999999994</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="25">
         <v>61.6</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="25">
         <v>73.900000000000006</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="37">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="41">
+      <c r="A22" s="34">
         <v>201</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="36">
         <v>72</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="25">
         <v>64.900000000000006</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="25">
         <v>78.2</v>
       </c>
-      <c r="H22" s="44">
+      <c r="H22" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="41">
+      <c r="A23" s="34">
         <v>202</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="36">
         <v>72</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="25">
         <v>64.900000000000006</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="25">
         <v>78.2</v>
       </c>
-      <c r="H23" s="44">
+      <c r="H23" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="41">
+      <c r="A24" s="34">
         <v>203</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="36">
         <v>69.099999999999994</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="25">
         <v>63.5</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="25">
         <v>74.2</v>
       </c>
-      <c r="H24" s="44">
+      <c r="H24" s="37">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="41">
+      <c r="A25" s="34">
         <v>204</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="36">
         <v>72.099999999999994</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="25">
         <v>65.599999999999994</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="25">
         <v>77.8</v>
       </c>
-      <c r="H25" s="44">
+      <c r="H25" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="41">
+      <c r="A26" s="34">
         <v>205</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="36">
         <v>66.900000000000006</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="25">
         <v>60.4</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="25">
         <v>72.900000000000006</v>
       </c>
-      <c r="H26" s="44">
+      <c r="H26" s="37">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="41">
+      <c r="A27" s="34">
         <v>206</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="36">
         <v>69.099999999999994</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="25">
         <v>63.5</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="25">
         <v>74.2</v>
       </c>
-      <c r="H27" s="44">
+      <c r="H27" s="37">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="41">
+      <c r="A28" s="34">
         <v>207</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="36">
         <v>67.099999999999994</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="25">
         <v>60.8</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="25">
         <v>72.900000000000006</v>
       </c>
-      <c r="H28" s="44">
+      <c r="H28" s="37">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="41">
+      <c r="A29" s="34">
         <v>208</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="36">
         <v>82.7</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="25">
         <v>76.900000000000006</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="25">
         <v>87.3</v>
       </c>
-      <c r="H29" s="44">
+      <c r="H29" s="37">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="41">
+      <c r="A30" s="34">
         <v>209</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="36">
         <v>72</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="25">
         <v>66.2</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="25">
         <v>77.099999999999994</v>
       </c>
-      <c r="H30" s="44">
+      <c r="H30" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="41">
+      <c r="A31" s="34">
         <v>210</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="36">
         <v>76.599999999999994</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="25">
         <v>70.2</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="25">
         <v>81.900000000000006</v>
       </c>
-      <c r="H31" s="44">
+      <c r="H31" s="37">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="41">
+      <c r="A32" s="34">
         <v>211</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="36">
         <v>80.3</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="25">
         <v>74.5</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="25">
         <v>85.1</v>
       </c>
-      <c r="H32" s="44">
+      <c r="H32" s="37">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="41">
+      <c r="A33" s="34">
         <v>212</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="36">
         <v>77.900000000000006</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="25">
         <v>72.599999999999994</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="25">
         <v>82.4</v>
       </c>
-      <c r="H33" s="44">
+      <c r="H33" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="41">
+      <c r="A34" s="34">
         <v>301</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="36">
         <v>79.099999999999994</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="25">
         <v>73.8</v>
       </c>
-      <c r="G34" s="27">
+      <c r="G34" s="25">
         <v>83.5</v>
       </c>
-      <c r="H34" s="44">
+      <c r="H34" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="41">
+      <c r="A35" s="34">
         <v>302</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="36">
         <v>86.3</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="25">
         <v>80.900000000000006</v>
       </c>
-      <c r="G35" s="27">
+      <c r="G35" s="25">
         <v>90.3</v>
       </c>
-      <c r="H35" s="44">
+      <c r="H35" s="37">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="41">
+      <c r="A36" s="34">
         <v>303</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="36">
         <v>76</v>
       </c>
-      <c r="F36" s="27">
+      <c r="F36" s="25">
         <v>70.599999999999994</v>
       </c>
-      <c r="G36" s="27">
+      <c r="G36" s="25">
         <v>80.599999999999994</v>
       </c>
-      <c r="H36" s="44">
+      <c r="H36" s="37">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="41">
+      <c r="A37" s="34">
         <v>304</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="36">
         <v>71.400000000000006</v>
       </c>
-      <c r="F37" s="27">
+      <c r="F37" s="25">
         <v>64.3</v>
       </c>
-      <c r="G37" s="27">
+      <c r="G37" s="25">
         <v>77.5</v>
       </c>
-      <c r="H37" s="44">
+      <c r="H37" s="37">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="41">
+      <c r="A38" s="34">
         <v>305</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="36">
         <v>70.2</v>
       </c>
-      <c r="F38" s="27">
+      <c r="F38" s="25">
         <v>63.1</v>
       </c>
-      <c r="G38" s="27">
+      <c r="G38" s="25">
         <v>76.400000000000006</v>
       </c>
-      <c r="H38" s="44">
+      <c r="H38" s="37">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="41">
+      <c r="A39" s="34">
         <v>306</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="36">
         <v>88.4</v>
       </c>
-      <c r="F39" s="27">
+      <c r="F39" s="25">
         <v>83.8</v>
       </c>
-      <c r="G39" s="27">
+      <c r="G39" s="25">
         <v>91.8</v>
       </c>
-      <c r="H39" s="44">
+      <c r="H39" s="37">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="41">
+      <c r="A40" s="34">
         <v>307</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="36">
         <v>73.599999999999994</v>
       </c>
-      <c r="F40" s="27">
+      <c r="F40" s="25">
         <v>67.400000000000006</v>
       </c>
-      <c r="G40" s="27">
+      <c r="G40" s="25">
         <v>79</v>
       </c>
-      <c r="H40" s="44">
+      <c r="H40" s="37">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="41">
+      <c r="A41" s="34">
         <v>308</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="43">
+      <c r="C41" s="36">
         <v>83.5</v>
       </c>
       <c r="D41" t="s">
         <v>107</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F41" s="25">
         <v>79</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="25">
         <v>87.2</v>
       </c>
-      <c r="H41" s="44">
+      <c r="H41" s="37">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="41">
+      <c r="A42" s="34">
         <v>309</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="43">
+      <c r="C42" s="36">
         <v>78</v>
       </c>
-      <c r="F42" s="27">
+      <c r="F42" s="25">
         <v>72.2</v>
       </c>
-      <c r="G42" s="27">
+      <c r="G42" s="25">
         <v>82.9</v>
       </c>
-      <c r="H42" s="44">
+      <c r="H42" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="41">
+      <c r="A43" s="34">
         <v>310</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43" s="36">
         <v>73.8</v>
       </c>
-      <c r="F43" s="27">
+      <c r="F43" s="25">
         <v>67.900000000000006</v>
       </c>
-      <c r="G43" s="27">
+      <c r="G43" s="25">
         <v>78.900000000000006</v>
       </c>
-      <c r="H43" s="44">
+      <c r="H43" s="37">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="41">
+      <c r="A44" s="34">
         <v>311</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="36">
         <v>65.400000000000006</v>
       </c>
-      <c r="F44" s="27">
+      <c r="F44" s="25">
         <v>59.6</v>
       </c>
-      <c r="G44" s="27">
+      <c r="G44" s="25">
         <v>70.7</v>
       </c>
-      <c r="H44" s="44">
+      <c r="H44" s="37">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="41">
+      <c r="A45" s="34">
         <v>312</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="36">
         <v>77.7</v>
       </c>
-      <c r="F45" s="27">
+      <c r="F45" s="25">
         <v>72.599999999999994</v>
       </c>
-      <c r="G45" s="27">
+      <c r="G45" s="25">
         <v>82.1</v>
       </c>
-      <c r="H45" s="44">
+      <c r="H45" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="41">
+      <c r="A46" s="34">
         <v>313</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="36">
         <v>69.7</v>
       </c>
-      <c r="F46" s="27">
+      <c r="F46" s="25">
         <v>63.6</v>
       </c>
-      <c r="G46" s="27">
+      <c r="G46" s="25">
         <v>75.099999999999994</v>
       </c>
-      <c r="H46" s="44">
+      <c r="H46" s="37">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="41">
+      <c r="A47" s="34">
         <v>314</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="36">
         <v>76.8</v>
       </c>
-      <c r="F47" s="27">
+      <c r="F47" s="25">
         <v>70.099999999999994</v>
       </c>
-      <c r="G47" s="27">
+      <c r="G47" s="25">
         <v>82.4</v>
       </c>
-      <c r="H47" s="44">
+      <c r="H47" s="37">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="41">
+      <c r="A48" s="34">
         <v>315</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="36">
         <v>69.900000000000006</v>
       </c>
-      <c r="F48" s="27">
+      <c r="F48" s="25">
         <v>64.400000000000006</v>
       </c>
-      <c r="G48" s="27">
+      <c r="G48" s="25">
         <v>74.900000000000006</v>
       </c>
-      <c r="H48" s="44">
+      <c r="H48" s="37">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="41">
+      <c r="A49" s="34">
         <v>316</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="36">
         <v>79.3</v>
       </c>
-      <c r="F49" s="27">
+      <c r="F49" s="25">
         <v>73.099999999999994</v>
       </c>
-      <c r="G49" s="27">
+      <c r="G49" s="25">
         <v>84.4</v>
       </c>
-      <c r="H49" s="44">
+      <c r="H49" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="41">
+      <c r="A50" s="34">
         <v>317</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="36">
         <v>83</v>
       </c>
-      <c r="F50" s="27">
+      <c r="F50" s="25">
         <v>77.400000000000006</v>
       </c>
-      <c r="G50" s="27">
+      <c r="G50" s="25">
         <v>87.5</v>
       </c>
-      <c r="H50" s="44">
+      <c r="H50" s="37">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="41">
+      <c r="A51" s="34">
         <v>318</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="36">
         <v>89.3</v>
       </c>
-      <c r="F51" s="27">
+      <c r="F51" s="25">
         <v>85.4</v>
       </c>
-      <c r="G51" s="27">
+      <c r="G51" s="25">
         <v>92.3</v>
       </c>
-      <c r="H51" s="44">
+      <c r="H51" s="37">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="41">
+      <c r="A52" s="34">
         <v>401</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52" s="36">
         <v>79.3</v>
       </c>
-      <c r="F52" s="27">
+      <c r="F52" s="25">
         <v>72.7</v>
       </c>
-      <c r="G52" s="27">
+      <c r="G52" s="25">
         <v>84.7</v>
       </c>
-      <c r="H52" s="44">
+      <c r="H52" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="41">
+      <c r="A53" s="34">
         <v>402</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B53" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="43">
+      <c r="C53" s="36">
         <v>79.099999999999994</v>
       </c>
-      <c r="F53" s="27">
+      <c r="F53" s="25">
         <v>72.599999999999994</v>
       </c>
-      <c r="G53" s="27">
+      <c r="G53" s="25">
         <v>84.4</v>
       </c>
-      <c r="H53" s="44">
+      <c r="H53" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="41">
+      <c r="A54" s="34">
         <v>403</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B54" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="43">
+      <c r="C54" s="36">
         <v>71.5</v>
       </c>
       <c r="D54" t="s">
         <v>107</v>
       </c>
-      <c r="F54" s="27">
+      <c r="F54" s="25">
         <v>65.599999999999994</v>
       </c>
-      <c r="G54" s="27">
+      <c r="G54" s="25">
         <v>76.7</v>
       </c>
-      <c r="H54" s="44">
+      <c r="H54" s="37">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="41">
+      <c r="A55" s="34">
         <v>404</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="36">
         <v>68.099999999999994</v>
       </c>
-      <c r="F55" s="27">
+      <c r="F55" s="25">
         <v>61.8</v>
       </c>
-      <c r="G55" s="27">
+      <c r="G55" s="25">
         <v>73.8</v>
       </c>
-      <c r="H55" s="44">
+      <c r="H55" s="37">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="41">
+      <c r="A56" s="34">
         <v>405</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="36">
         <v>78.400000000000006</v>
       </c>
-      <c r="F56" s="27">
+      <c r="F56" s="25">
         <v>71.7</v>
       </c>
-      <c r="G56" s="27">
+      <c r="G56" s="25">
         <v>83.9</v>
       </c>
-      <c r="H56" s="44">
+      <c r="H56" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="41">
+      <c r="A57" s="34">
         <v>406</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="43">
+      <c r="C57" s="36">
         <v>82</v>
       </c>
-      <c r="F57" s="27">
+      <c r="F57" s="25">
         <v>77.099999999999994</v>
       </c>
-      <c r="G57" s="27">
+      <c r="G57" s="25">
         <v>86</v>
       </c>
-      <c r="H57" s="44">
+      <c r="H57" s="37">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="41">
+      <c r="A58" s="34">
         <v>407</v>
       </c>
-      <c r="B58" s="42" t="s">
+      <c r="B58" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C58" s="43">
+      <c r="C58" s="36">
         <v>71.099999999999994</v>
       </c>
-      <c r="F58" s="27">
+      <c r="F58" s="25">
         <v>65.599999999999994</v>
       </c>
-      <c r="G58" s="27">
+      <c r="G58" s="25">
         <v>76.099999999999994</v>
       </c>
-      <c r="H58" s="44">
+      <c r="H58" s="37">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="41">
+      <c r="A59" s="34">
         <v>408</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="B59" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="43">
+      <c r="C59" s="36">
         <v>79.099999999999994</v>
       </c>
-      <c r="F59" s="27">
+      <c r="F59" s="25">
         <v>72.7</v>
       </c>
-      <c r="G59" s="27">
+      <c r="G59" s="25">
         <v>84.4</v>
       </c>
-      <c r="H59" s="44">
+      <c r="H59" s="37">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="41">
+      <c r="A60" s="34">
         <v>409</v>
       </c>
-      <c r="B60" s="42" t="s">
+      <c r="B60" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="43">
+      <c r="C60" s="36">
         <v>77.8</v>
       </c>
-      <c r="F60" s="27">
+      <c r="F60" s="25">
         <v>71.5</v>
       </c>
-      <c r="G60" s="27">
+      <c r="G60" s="25">
         <v>83.1</v>
       </c>
-      <c r="H60" s="44">
+      <c r="H60" s="37">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="41">
+      <c r="A61" s="34">
         <v>410</v>
       </c>
-      <c r="B61" s="42" t="s">
+      <c r="B61" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="43">
+      <c r="C61" s="36">
         <v>77</v>
       </c>
-      <c r="F61" s="27">
+      <c r="F61" s="25">
         <v>70.7</v>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="25">
         <v>82.3</v>
       </c>
-      <c r="H61" s="44">
+      <c r="H61" s="37">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="41">
+      <c r="A62" s="34">
         <v>411</v>
       </c>
-      <c r="B62" s="42" t="s">
+      <c r="B62" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="43">
+      <c r="C62" s="36">
         <v>85.7</v>
       </c>
-      <c r="F62" s="27">
+      <c r="F62" s="25">
         <v>81</v>
       </c>
-      <c r="G62" s="27">
+      <c r="G62" s="25">
         <v>89.4</v>
       </c>
-      <c r="H62" s="44">
+      <c r="H62" s="37">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="41">
+      <c r="A63" s="34">
         <v>412</v>
       </c>
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C63" s="43">
+      <c r="C63" s="36">
         <v>81.900000000000006</v>
       </c>
-      <c r="F63" s="27">
+      <c r="F63" s="25">
         <v>76.400000000000006</v>
       </c>
-      <c r="G63" s="27">
+      <c r="G63" s="25">
         <v>86.4</v>
       </c>
-      <c r="H63" s="44">
+      <c r="H63" s="37">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="41">
+      <c r="A64" s="34">
         <v>413</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="43">
+      <c r="C64" s="36">
         <v>74.400000000000006</v>
       </c>
-      <c r="F64" s="27">
+      <c r="F64" s="25">
         <v>66.3</v>
       </c>
-      <c r="G64" s="27">
+      <c r="G64" s="25">
         <v>81.099999999999994</v>
       </c>
-      <c r="H64" s="44">
+      <c r="H64" s="37">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="41">
+      <c r="A65" s="34">
         <v>414</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C65" s="43">
+      <c r="C65" s="36">
         <v>75.5</v>
       </c>
       <c r="D65" t="s">
         <v>108</v>
       </c>
-      <c r="F65" s="27">
+      <c r="F65" s="25">
         <v>69.2</v>
       </c>
-      <c r="G65" s="27">
+      <c r="G65" s="25">
         <v>80.8</v>
       </c>
-      <c r="H65" s="44">
+      <c r="H65" s="37">
         <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="41">
+      <c r="A66" s="34">
         <v>501</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C66" s="43">
+      <c r="C66" s="36">
         <v>77</v>
       </c>
-      <c r="F66" s="27">
+      <c r="F66" s="25">
         <v>70.2</v>
       </c>
-      <c r="G66" s="27">
+      <c r="G66" s="25">
         <v>82.7</v>
       </c>
-      <c r="H66" s="44">
+      <c r="H66" s="37">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="41">
+      <c r="A67" s="34">
         <v>502</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C67" s="43">
+      <c r="C67" s="36">
         <v>75.5</v>
       </c>
       <c r="D67" t="s">
         <v>107</v>
       </c>
-      <c r="F67" s="27">
+      <c r="F67" s="25">
         <v>66.3</v>
       </c>
-      <c r="G67" s="27">
+      <c r="G67" s="25">
         <v>82.9</v>
       </c>
-      <c r="H67" s="44">
+      <c r="H67" s="37">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="45">
+      <c r="A68" s="38">
         <v>503</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C68" s="47">
+      <c r="C68" s="40">
         <v>87.7</v>
       </c>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="49">
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="42">
         <v>82.9</v>
       </c>
-      <c r="G68" s="49">
+      <c r="G68" s="42">
         <v>91.3</v>
       </c>
-      <c r="H68" s="50">
+      <c r="H68" s="43">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="H69" s="27"/>
+      <c r="H69" s="25"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="H70" s="27"/>
+      <c r="H70" s="25"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="51" t="s">
+      <c r="A71" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="B71" s="52" t="s">
+      <c r="B71" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="C71" s="53" t="s">
+      <c r="C71" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54" t="s">
+      <c r="D71" s="47"/>
+      <c r="E71" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F71" s="53" t="s">
+      <c r="F71" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G71" s="40" t="s">
+      <c r="G71" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H71" s="55" t="s">
+      <c r="H71" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="41">
+      <c r="A72" s="34">
         <v>2</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C72" s="27">
+      <c r="C72" s="25">
         <v>73.400000000000006</v>
       </c>
-      <c r="F72" s="27">
+      <c r="F72" s="25">
         <v>71.400000000000006</v>
       </c>
-      <c r="G72" s="56">
+      <c r="G72" s="49">
         <v>75.3</v>
       </c>
-      <c r="H72" s="67">
+      <c r="H72" s="60">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="41">
+      <c r="A73" s="34">
         <v>3</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="C73" s="27">
+      <c r="C73" s="25">
         <v>76.900000000000006</v>
       </c>
-      <c r="F73" s="27">
+      <c r="F73" s="25">
         <v>75.599999999999994</v>
       </c>
-      <c r="G73" s="56">
+      <c r="G73" s="49">
         <v>78.2</v>
       </c>
-      <c r="H73" s="57">
+      <c r="H73" s="50">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="41">
+      <c r="A74" s="34">
         <v>1</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="27">
+      <c r="C74" s="25">
         <v>83.2</v>
       </c>
-      <c r="F74" s="27">
+      <c r="F74" s="25">
         <v>81.5</v>
       </c>
-      <c r="G74" s="56">
+      <c r="G74" s="49">
         <v>84.8</v>
       </c>
-      <c r="H74" s="57">
+      <c r="H74" s="50">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="41">
+      <c r="A75" s="34">
         <v>4</v>
       </c>
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C75" s="27">
+      <c r="C75" s="25">
         <v>76.400000000000006</v>
       </c>
-      <c r="F75" s="27">
+      <c r="F75" s="25">
         <v>74.7</v>
       </c>
-      <c r="G75" s="56">
+      <c r="G75" s="49">
         <v>78</v>
       </c>
-      <c r="H75" s="57">
+      <c r="H75" s="50">
         <f t="shared" ref="H75:H80" si="1">ROUND(C75,0)</f>
         <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="45">
+      <c r="A76" s="38">
         <v>5</v>
       </c>
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="49">
+      <c r="C76" s="42">
         <v>81.099999999999994</v>
       </c>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="49">
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
+      <c r="F76" s="42">
         <v>77.400000000000006</v>
       </c>
-      <c r="G76" s="58">
+      <c r="G76" s="51">
         <v>84.4</v>
       </c>
-      <c r="H76" s="59">
+      <c r="H76" s="52">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="H77" s="27"/>
+      <c r="H77" s="25"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="H78" s="27"/>
+      <c r="H78" s="25"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="B79" s="60" t="s">
+      <c r="B79" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C79" s="53" t="s">
+      <c r="C79" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D79" s="54"/>
-      <c r="E79" s="54" t="s">
+      <c r="D79" s="47"/>
+      <c r="E79" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="F79" s="53" t="s">
+      <c r="F79" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G79" s="40" t="s">
+      <c r="G79" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H79" s="55" t="s">
+      <c r="H79" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:8">
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C80" s="61">
+      <c r="C80" s="54">
         <v>77.8</v>
       </c>
-      <c r="D80" s="62"/>
-      <c r="E80" s="62"/>
-      <c r="F80" s="61">
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="54">
         <v>77</v>
       </c>
-      <c r="G80" s="63">
+      <c r="G80" s="56">
         <v>78.599999999999994</v>
       </c>
-      <c r="H80" s="64">
+      <c r="H80" s="57">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
@@ -10795,6 +10793,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="4eab1d2f-0a6f-43b5-bd47-0cc182e7f81d" xsi:nil="true"/>
@@ -10803,15 +10810,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10834,6 +10832,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6697668-EC76-46C6-A886-FE46F18A5C65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBDC9F0A-70B2-4955-92FB-558444EE0082}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10842,12 +10848,4 @@
     <ds:schemaRef ds:uri="18262a4b-7b39-4d27-b1ee-8cb22edac4a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6697668-EC76-46C6-A886-FE46F18A5C65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>